<commit_message>
Selenium season -3 as on May 30th
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/excels/Master_TestData.xlsx
+++ b/src/test/resources/testdata/excels/Master_TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FLM19thFebWS\FrameWorkAutomation\src\test\resources\testdata\excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14129399-8EF4-45EA-940A-0FC37ABC7B1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{025DF3C3-0D7E-4598-9EC4-CAB46E66BACD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1416" yWindow="1128" windowWidth="21624" windowHeight="11112" xr2:uid="{E1DB891E-4724-4F90-B920-9B3042ED20AF}"/>
   </bookViews>
@@ -459,7 +459,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="25.8" x14ac:dyDescent="0.5"/>

</xml_diff>